<commit_message>
added antenna to REV10 BOM
</commit_message>
<xml_diff>
--- a/Arduino/hardware/REV10/BOM.xlsx
+++ b/Arduino/hardware/REV10/BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="186">
   <si>
     <t># of boards ttl</t>
   </si>
@@ -331,6 +331,9 @@
     <t>712-5320</t>
   </si>
   <si>
+    <t>RS</t>
+  </si>
+  <si>
     <t>84mm* of insulated semi-flexible antenna wire (~0.33sqmm). *Depends on PCB track length.</t>
   </si>
   <si>
@@ -532,10 +535,10 @@
     <t>?</t>
   </si>
   <si>
-    <t>100?</t>
-  </si>
-  <si>
     <t>SIM900 shield</t>
+  </si>
+  <si>
+    <t>Link??</t>
   </si>
   <si>
     <t>Total:</t>
@@ -576,7 +579,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -630,6 +633,12 @@
     <font>
       <u/>
       <color rgb="FF6AA84F"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -694,7 +703,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="66">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
@@ -812,22 +821,40 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -840,12 +867,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -866,13 +893,13 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1006,7 +1033,7 @@
         <v>0.342</v>
       </c>
       <c r="E5" s="16" t="str">
-        <f t="shared" ref="E5:E20" si="2">D5*B5</f>
+        <f t="shared" ref="E5:E33" si="2">D5*B5</f>
         <v>34.2</v>
       </c>
       <c r="F5" s="19" t="s">
@@ -1632,32 +1659,41 @@
       </c>
     </row>
     <row r="21" ht="12.0" customHeight="1">
-      <c r="A21" s="15">
-        <v>1.0</v>
+      <c r="A21" s="39">
+        <v>0.001</v>
       </c>
       <c r="B21" s="16" t="str">
         <f t="shared" si="3"/>
-        <v>100</v>
-      </c>
-      <c r="C21" s="37"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="19" t="s">
+        <v>0.1</v>
+      </c>
+      <c r="C21" s="40">
+        <v>1000.0</v>
+      </c>
+      <c r="D21" s="41">
+        <v>11.99</v>
+      </c>
+      <c r="E21" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>1.199</v>
+      </c>
+      <c r="F21" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="15" t="s">
+      <c r="G21" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="J21" s="15" t="s">
+      <c r="H21" s="43"/>
+      <c r="I21" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="K21" s="22" t="s">
+      <c r="J21" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="K21" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="L21" s="20" t="s">
-        <v>108</v>
+      <c r="L21" s="46" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="22" ht="12.0" customHeight="1">
@@ -1675,29 +1711,29 @@
         <v>2.53</v>
       </c>
       <c r="E22" s="16" t="str">
-        <f t="shared" ref="E22:E33" si="4">D22*B22</f>
+        <f t="shared" si="2"/>
         <v>253</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J22" s="15" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="K22" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="L22" s="41" t="s">
-        <v>114</v>
+      <c r="L22" s="47" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="23" ht="12.0" customHeight="1">
@@ -1715,29 +1751,29 @@
         <v>3.6</v>
       </c>
       <c r="E23" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>360</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G23" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="H23" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="H23" s="15" t="s">
-        <v>115</v>
-      </c>
       <c r="I23" s="15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="L23" s="41" t="s">
         <v>120</v>
+      </c>
+      <c r="L23" s="47" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="24" ht="12.0" customHeight="1">
@@ -1755,29 +1791,29 @@
         <v>1.008</v>
       </c>
       <c r="E24" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>100.8</v>
       </c>
       <c r="F24" s="21">
         <v>4681350.0</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H24" s="23" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K24" s="15" t="s">
         <v>20</v>
       </c>
       <c r="L24" s="24" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" ht="12.0" customHeight="1">
@@ -1795,29 +1831,29 @@
         <v>6.21</v>
       </c>
       <c r="E25" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>621</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G25" s="35" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H25" s="23" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L25" s="24" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" ht="12.0" customHeight="1">
@@ -1835,7 +1871,7 @@
         <v>0.561</v>
       </c>
       <c r="E26" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>56.1</v>
       </c>
       <c r="F26" s="23">
@@ -1845,19 +1881,19 @@
         <v>35</v>
       </c>
       <c r="H26" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="K26" s="5" t="s">
         <v>98</v>
       </c>
       <c r="L26" s="24" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" ht="12.0" customHeight="1">
@@ -1875,29 +1911,29 @@
         <v>0.062</v>
       </c>
       <c r="E27" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>6.2</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G27" s="23" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H27" s="23" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="K27" s="15" t="s">
         <v>20</v>
       </c>
       <c r="L27" s="24" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" ht="12.0" customHeight="1">
@@ -1915,29 +1951,29 @@
         <v>0.008</v>
       </c>
       <c r="E28" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G28" s="23" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H28" s="23" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K28" s="15" t="s">
         <v>20</v>
       </c>
       <c r="L28" s="24" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" ht="12.0" customHeight="1">
@@ -1955,29 +1991,29 @@
         <v>0.413</v>
       </c>
       <c r="E29" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>82.6</v>
       </c>
       <c r="F29" s="23" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G29" s="15" t="s">
         <v>35</v>
       </c>
       <c r="H29" s="23" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="K29" s="15" t="s">
         <v>20</v>
       </c>
       <c r="L29" s="24" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" ht="12.0" customHeight="1">
@@ -1995,29 +2031,29 @@
         <v>0.346</v>
       </c>
       <c r="E30" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>34.6</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G30" s="15" t="s">
         <v>35</v>
       </c>
       <c r="H30" s="23" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K30" s="15" t="s">
         <v>20</v>
       </c>
       <c r="L30" s="24" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" ht="12.0" customHeight="1">
@@ -2035,29 +2071,29 @@
         <v>0.287</v>
       </c>
       <c r="E31" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>57.4</v>
       </c>
-      <c r="F31" s="42">
+      <c r="F31" s="48">
         <v>1593478.0</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H31" s="43" t="s">
         <v>160</v>
       </c>
+      <c r="H31" s="49" t="s">
+        <v>161</v>
+      </c>
       <c r="I31" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K31" s="5" t="s">
         <v>98</v>
       </c>
       <c r="L31" s="24" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="32" ht="12.0" customHeight="1">
@@ -2075,29 +2111,29 @@
         <v>0.561</v>
       </c>
       <c r="E32" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>56.1</v>
       </c>
       <c r="F32" s="21">
         <v>1593462.0</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K32" s="5" t="s">
         <v>98</v>
       </c>
       <c r="L32" s="24" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="33" ht="12.0" customHeight="1">
@@ -2115,63 +2151,64 @@
         <v>0.375</v>
       </c>
       <c r="E33" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>37.5</v>
       </c>
       <c r="F33" s="21">
         <v>7991959.0</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="H33" s="44" t="s">
         <v>168</v>
       </c>
+      <c r="H33" s="50" t="s">
+        <v>169</v>
+      </c>
       <c r="I33" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K33" s="5" t="s">
         <v>98</v>
       </c>
       <c r="L33" s="24" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34" ht="12.0" customHeight="1">
       <c r="A34" s="1">
         <v>1.0</v>
       </c>
-      <c r="B34" s="45" t="str">
+      <c r="B34" s="51" t="str">
         <f>'BOM - Main'!B$1*A34</f>
         <v>100</v>
       </c>
       <c r="C34" s="8"/>
-      <c r="D34" s="46"/>
+      <c r="D34" s="52"/>
       <c r="E34" s="16"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="L34" s="47"/>
+        <v>173</v>
+      </c>
+      <c r="L34" s="53"/>
     </row>
     <row r="35" ht="12.0" customHeight="1">
       <c r="A35" s="2">
         <v>1.0</v>
       </c>
-      <c r="B35" s="48" t="s">
-        <v>173</v>
+      <c r="B35" s="51" t="str">
+        <f>'BOM - Main'!B$1*A35</f>
+        <v>100</v>
       </c>
       <c r="C35" s="8"/>
-      <c r="D35" s="46"/>
+      <c r="D35" s="52"/>
       <c r="E35" s="8"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
@@ -2181,20 +2218,22 @@
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="L35" s="47"/>
+        <v>173</v>
+      </c>
+      <c r="L35" s="54" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="36" ht="12.0" customHeight="1">
       <c r="A36" s="1"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
-      <c r="D36" s="49" t="s">
-        <v>175</v>
-      </c>
-      <c r="E36" s="45" t="str">
+      <c r="D36" s="55" t="s">
+        <v>176</v>
+      </c>
+      <c r="E36" s="51" t="str">
         <f>SUM(E5:E34)</f>
-        <v>2160.4</v>
+        <v>2161.599</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
@@ -2202,18 +2241,18 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
-      <c r="L36" s="47"/>
+      <c r="L36" s="53"/>
     </row>
     <row r="37" ht="12.0" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
-      <c r="D37" s="49" t="s">
-        <v>176</v>
-      </c>
-      <c r="E37" s="45" t="str">
+      <c r="D37" s="55" t="s">
+        <v>177</v>
+      </c>
+      <c r="E37" s="51" t="str">
         <f>E36/B1</f>
-        <v>21.604</v>
+        <v>21.61599</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
@@ -2221,62 +2260,62 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
-      <c r="L37" s="47"/>
+      <c r="L37" s="53"/>
     </row>
     <row r="38" ht="12.0" customHeight="1">
-      <c r="A38" s="50" t="s">
-        <v>177</v>
+      <c r="A38" s="56" t="s">
+        <v>178</v>
       </c>
       <c r="B38" s="37"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="52"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="54"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="55"/>
-      <c r="K38" s="55"/>
-      <c r="L38" s="56"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="59"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="61"/>
+      <c r="H38" s="61"/>
+      <c r="I38" s="61"/>
+      <c r="J38" s="61"/>
+      <c r="K38" s="61"/>
+      <c r="L38" s="62"/>
     </row>
     <row r="39" ht="12.0" customHeight="1">
-      <c r="A39" s="55">
+      <c r="A39" s="61">
         <v>1.0</v>
       </c>
       <c r="B39" s="16" t="str">
-        <f t="shared" ref="B39:B40" si="5">B$1*A39</f>
+        <f t="shared" ref="B39:B40" si="4">B$1*A39</f>
         <v>100</v>
       </c>
-      <c r="C39" s="51">
+      <c r="C39" s="57">
         <v>5.0</v>
       </c>
-      <c r="D39" s="52">
+      <c r="D39" s="58">
         <v>0.71</v>
       </c>
-      <c r="E39" s="53" t="str">
-        <f t="shared" ref="E39:E40" si="6">D39*B39</f>
+      <c r="E39" s="59" t="str">
+        <f t="shared" ref="E39:E40" si="5">D39*B39</f>
         <v>71</v>
       </c>
-      <c r="F39" s="54" t="s">
-        <v>178</v>
-      </c>
-      <c r="G39" s="55" t="s">
+      <c r="F39" s="60" t="s">
+        <v>179</v>
+      </c>
+      <c r="G39" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="H39" s="55" t="s">
-        <v>179</v>
-      </c>
-      <c r="I39" s="55" t="s">
+      <c r="H39" s="61" t="s">
+        <v>180</v>
+      </c>
+      <c r="I39" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="J39" s="55" t="s">
+      <c r="J39" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="K39" s="55" t="s">
+      <c r="K39" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="L39" s="57" t="s">
-        <v>180</v>
+      <c r="L39" s="63" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="40" ht="12.0" customHeight="1">
@@ -2284,39 +2323,39 @@
         <v>2.0</v>
       </c>
       <c r="B40" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>200</v>
+      </c>
+      <c r="C40" s="57">
+        <v>100.0</v>
+      </c>
+      <c r="D40" s="58">
+        <v>0.127</v>
+      </c>
+      <c r="E40" s="59" t="str">
         <f t="shared" si="5"/>
-        <v>200</v>
-      </c>
-      <c r="C40" s="51">
-        <v>100.0</v>
-      </c>
-      <c r="D40" s="52">
-        <v>0.127</v>
-      </c>
-      <c r="E40" s="53" t="str">
-        <f t="shared" si="6"/>
         <v>25.4</v>
       </c>
-      <c r="F40" s="58" t="s">
-        <v>181</v>
+      <c r="F40" s="64" t="s">
+        <v>182</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="H40" s="58" t="s">
         <v>183</v>
       </c>
-      <c r="I40" s="55" t="s">
+      <c r="H40" s="64" t="s">
+        <v>184</v>
+      </c>
+      <c r="I40" s="61" t="s">
         <v>96</v>
       </c>
       <c r="J40" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="K40" s="55" t="s">
+      <c r="K40" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="L40" s="59" t="s">
-        <v>184</v>
+      <c r="L40" s="65" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>